<commit_message>
ActionCondition 테스트 및 수정
클립의 루프 여부 판정이 빗나가는 경우 있음 -> 판정 방식 자체를 clip info 기반으로 변경 및 clip info length가 0일 땐 무시
attack 조건의 경우 입력 프레임에만 0이 들어와야 데이터 시나리오대로 동작해서 다시 key down으로 롤백
기타) action 전환 최적화, 한 update 안에서 마지막으로 결정한 한 액션으로만 전환되도록
</commit_message>
<xml_diff>
--- a/RunInBoots/Assets/Excel/ActionTable.xlsx
+++ b/RunInBoots/Assets/Excel/ActionTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paul1\OneDrive\문서\Git\team-project-for-2024-fall-swpp-team-05\RunInBoots\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBB48525-978E-4252-AA25-F23866AC9AC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7707E27F-CD63-4763-BA93-7D52AC5B63C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-165" windowWidth="29040" windowHeight="15720" xr2:uid="{D47B4964-B3F8-4260-96F1-09DFF1E3D63F}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="158">
   <si>
     <t>Key</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -645,7 +645,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -660,12 +660,6 @@
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1115,7 +1109,7 @@
   <dimension ref="A1:AQ38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z16" sqref="Z16"/>
+      <selection activeCell="T11" sqref="T11:W11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1439,7 +1433,7 @@
   IF(표1[[#This Row],[_Condition4]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition4]] &amp; "," &amp; 표1[[#This Row],[_CParam4]] &amp; "," &amp; 표1[[#This Row],[_Function4]] &amp; "," &amp; 표1[[#This Row],[_FParam4]] &amp; "}", ""),
   IF(표1[[#This Row],[_Condition5]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition5]] &amp; "," &amp; 표1[[#This Row],[_CParam5]] &amp; "," &amp; 표1[[#This Row],[_Function5]] &amp; "," &amp; 표1[[#This Row],[_FParam5]] &amp; "}", ""),  IF(표1[[#This Row],[_Condition6]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition6]] &amp; "," &amp; 표1[[#This Row],[_CParam6]] &amp; "," &amp; 표1[[#This Row],[_Function6]] &amp; "," &amp; 표1[[#This Row],[_FParam6]] &amp; "}", ""),  IF(표1[[#This Row],[_Condition7]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition7]] &amp; "," &amp; 표1[[#This Row],[_CParam7]] &amp; "," &amp; 표1[[#This Row],[_Function7]] &amp; "," &amp; 표1[[#This Row],[_FParam7]] &amp; "}", ""),  IF(표1[[#This Row],[_Condition8]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition8]] &amp; "," &amp; 표1[[#This Row],[_CParam8]] &amp; "," &amp; 표1[[#This Row],[_Function8]] &amp; "," &amp; 표1[[#This Row],[_FParam8]] &amp; "}", "")
 ) &amp; "]"</f>
-        <v>[{InputX,1,MoveInputX,1},{InputX,0,SetAction,101},{InputY,-1,SetAction,103},{InputY,1,SetAction,108},{Attack,1,SetAction,106},{Run,1,SetAction,107},{OnLand,0,SetAction,105},{JumpValid,1,SetAction,104}]</v>
+        <v>[{InputX,1,MoveInputX,1},{InputX,0,SetAction,101},{InputY,-1,SetAction,103},{InputY,1,SetAction,108},{Run,1,SetAction,107},{Attack,1,SetAction,106},{OnLand,0,SetAction,105},{JumpValid,1,SetAction,104}]</v>
       </c>
       <c r="L3" t="s">
         <v>36</v>
@@ -1490,28 +1484,28 @@
         <v>108</v>
       </c>
       <c r="AB3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC3">
+        <v>1</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE3">
+        <v>107</v>
+      </c>
+      <c r="AF3" t="s">
         <v>46</v>
       </c>
-      <c r="AC3">
-        <v>1</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>72</v>
-      </c>
-      <c r="AE3">
+      <c r="AG3">
+        <v>1</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AI3">
         <v>106</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>48</v>
-      </c>
-      <c r="AG3">
-        <v>1</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>72</v>
-      </c>
-      <c r="AI3">
-        <v>107</v>
       </c>
       <c r="AJ3" t="s">
         <v>50</v>
@@ -1904,7 +1898,7 @@
   IF(표1[[#This Row],[_Condition4]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition4]] &amp; "," &amp; 표1[[#This Row],[_CParam4]] &amp; "," &amp; 표1[[#This Row],[_Function4]] &amp; "," &amp; 표1[[#This Row],[_FParam4]] &amp; "}", ""),
   IF(표1[[#This Row],[_Condition5]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition5]] &amp; "," &amp; 표1[[#This Row],[_CParam5]] &amp; "," &amp; 표1[[#This Row],[_Function5]] &amp; "," &amp; 표1[[#This Row],[_FParam5]] &amp; "}", ""),  IF(표1[[#This Row],[_Condition6]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition6]] &amp; "," &amp; 표1[[#This Row],[_CParam6]] &amp; "," &amp; 표1[[#This Row],[_Function6]] &amp; "," &amp; 표1[[#This Row],[_FParam6]] &amp; "}", ""),  IF(표1[[#This Row],[_Condition7]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition7]] &amp; "," &amp; 표1[[#This Row],[_CParam7]] &amp; "," &amp; 표1[[#This Row],[_Function7]] &amp; "," &amp; 표1[[#This Row],[_FParam7]] &amp; "}", ""),  IF(표1[[#This Row],[_Condition8]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition8]] &amp; "," &amp; 표1[[#This Row],[_CParam8]] &amp; "," &amp; 표1[[#This Row],[_Function8]] &amp; "," &amp; 표1[[#This Row],[_FParam8]] &amp; "}", "")
 ) &amp; "]"</f>
-        <v>[{InputX,1,MoveInputX,2},{Attack,0,SetAction,102},{InputX,0,SetAction,101},{InputY,-1,SetAction,103},{InputY,1,SetAction,108},{OnLand,0,SetAction,105},{JumpValid,1,SetAction,104}]</v>
+        <v>[{InputX,1,MoveInputX,2},{Run,0,SetAction,102},{InputX,0,SetAction,101},{InputY,-1,SetAction,103},{InputY,1,SetAction,108},{OnLand,0,SetAction,105},{JumpValid,1,SetAction,104}]</v>
       </c>
       <c r="L8" t="s">
         <v>36</v>
@@ -1919,7 +1913,7 @@
         <v>2</v>
       </c>
       <c r="P8" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="Q8">
         <v>0</v>
@@ -2201,7 +2195,7 @@
   IF(표1[[#This Row],[_Condition4]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition4]] &amp; "," &amp; 표1[[#This Row],[_CParam4]] &amp; "," &amp; 표1[[#This Row],[_Function4]] &amp; "," &amp; 표1[[#This Row],[_FParam4]] &amp; "}", ""),
   IF(표1[[#This Row],[_Condition5]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition5]] &amp; "," &amp; 표1[[#This Row],[_CParam5]] &amp; "," &amp; 표1[[#This Row],[_Function5]] &amp; "," &amp; 표1[[#This Row],[_FParam5]] &amp; "}", ""),  IF(표1[[#This Row],[_Condition6]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition6]] &amp; "," &amp; 표1[[#This Row],[_CParam6]] &amp; "," &amp; 표1[[#This Row],[_Function6]] &amp; "," &amp; 표1[[#This Row],[_FParam6]] &amp; "}", ""),  IF(표1[[#This Row],[_Condition7]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition7]] &amp; "," &amp; 표1[[#This Row],[_CParam7]] &amp; "," &amp; 표1[[#This Row],[_Function7]] &amp; "," &amp; 표1[[#This Row],[_FParam7]] &amp; "}", ""),  IF(표1[[#This Row],[_Condition8]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition8]] &amp; "," &amp; 표1[[#This Row],[_CParam8]] &amp; "," &amp; 표1[[#This Row],[_Function8]] &amp; "," &amp; 표1[[#This Row],[_FParam8]] &amp; "}", "")
 ) &amp; "]"</f>
-        <v>[{InputX,1,MoveInputX,1},{InputX,0,SetAction,103},{Attack,1,SetAction,133},{OnLand,0,SetAction,105},{JumpValid,1,SetAction,134}]</v>
+        <v>[{InputX,1,MoveInputX,1},{InputX,0,SetAction,103},{Risable,1,SetAction,101},{Attack,1,SetAction,133},{OnLand,0,SetAction,105},{JumpValid,1,SetAction,134}]</v>
       </c>
       <c r="L11" t="s">
         <v>36</v>
@@ -2228,39 +2222,51 @@
         <v>103</v>
       </c>
       <c r="T11" t="s">
+        <v>40</v>
+      </c>
+      <c r="U11">
+        <v>1</v>
+      </c>
+      <c r="V11" t="s">
+        <v>72</v>
+      </c>
+      <c r="W11">
+        <v>101</v>
+      </c>
+      <c r="X11" t="s">
         <v>46</v>
       </c>
-      <c r="U11">
-        <v>1</v>
-      </c>
-      <c r="V11" t="s">
-        <v>72</v>
-      </c>
-      <c r="W11">
+      <c r="Y11">
+        <v>1</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA11">
         <v>133</v>
       </c>
-      <c r="X11" t="s">
+      <c r="AB11" t="s">
         <v>50</v>
       </c>
-      <c r="Y11">
-        <v>0</v>
-      </c>
-      <c r="Z11" t="s">
-        <v>72</v>
-      </c>
-      <c r="AA11">
+      <c r="AC11">
+        <v>0</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE11">
         <v>105</v>
       </c>
-      <c r="AB11" t="s">
+      <c r="AF11" t="s">
         <v>44</v>
       </c>
-      <c r="AC11">
-        <v>1</v>
-      </c>
-      <c r="AD11" t="s">
-        <v>72</v>
-      </c>
-      <c r="AE11">
+      <c r="AG11">
+        <v>1</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>72</v>
+      </c>
+      <c r="AI11">
         <v>134</v>
       </c>
     </row>
@@ -2345,6 +2351,9 @@
       </c>
       <c r="I13">
         <v>0.1</v>
+      </c>
+      <c r="J13">
+        <v>101</v>
       </c>
       <c r="K13" t="str">
         <f>"[" &amp; _xlfn.TEXTJOIN(",", TRUE,
@@ -4078,13 +4087,13 @@
           <x14:formula1>
             <xm:f>_helper!$B:$B</xm:f>
           </x14:formula1>
-          <xm:sqref>AP3 AL8 AL2:AL3 N2:N38 AH2:AH38 AD2:AD38 Z2:Z38 R2:R38 V2:V38</xm:sqref>
+          <xm:sqref>AP3 AL8 AL2:AL3 N2:N38 AH2:AH38 R2:R38 AD2:AD38 Z2:Z38 V2:V38</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{38EFAF22-778F-4724-863A-ECD1104B256A}">
           <x14:formula1>
             <xm:f>_helper!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>AN3 AJ8 AJ2:AJ3 AF2:AF38 L2:L38 AB2:AB38 X2:X38 P2:P38 T2:T38</xm:sqref>
+          <xm:sqref>AN3 AJ8 AJ2:AJ3 AF2:AF38 L2:L38 P2:P38 AB2:AB38 X2:X38 T2:T38</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
[TASK-P54] Stage2 완성 및 MoveBlockManager 코드 이슈로 인해 예전 코드로 롤백
MoveBlockManager : 갱신 시점 맞추기로 별도 처리 없이 블록 위 PC와 함께 이동했던 것으로 기억하나, 가로 이동 시 PC 두고 가는 이슈 재현됨. 예전 수정 코드 복원으로 해결
</commit_message>
<xml_diff>
--- a/RunInBoots/Assets/Excel/ActionTable.xlsx
+++ b/RunInBoots/Assets/Excel/ActionTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paul1\OneDrive\문서\Git\team-project-for-2024-fall-swpp-team-05\RunInBoots\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{655D3544-0520-465C-9D36-0FEB322747A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F14FC528-358E-452D-8DA7-31319F60FE8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D47B4964-B3F8-4260-96F1-09DFF1E3D63F}"/>
   </bookViews>
@@ -1129,8 +1129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{315677FB-260A-4651-8343-EA147A10AE96}">
   <dimension ref="A1:AQ38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H24"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3373,10 +3373,10 @@
         <v>152</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E25">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="F25">
         <v>0.1</v>
@@ -3424,7 +3424,7 @@
         <v>153</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E26">
         <v>0</v>

</xml_diff>

<commit_message>
[TASK-P54] Stage3 제작 및 TigerHat 조정
TigerHat 관련 => 도망 사거리 증가, 매 프레임 도망 액션 해제 반복하던 로직 오류 수정
</commit_message>
<xml_diff>
--- a/RunInBoots/Assets/Excel/ActionTable.xlsx
+++ b/RunInBoots/Assets/Excel/ActionTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paul1\OneDrive\문서\Git\team-project-for-2024-fall-swpp-team-05\RunInBoots\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A843F95-6409-4975-A61A-5891C308B65E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC5FE762-58AF-4DC9-A188-5B2390876D07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D47B4964-B3F8-4260-96F1-09DFF1E3D63F}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="166">
   <si>
     <t>Key</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -659,6 +659,14 @@
   </si>
   <si>
     <t>None</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>경비견 도망</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dog_runaway</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -743,8 +751,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{07CD4AC0-49C4-4B86-80BF-22BA39ABB725}" name="표1" displayName="표1" ref="A1:AQ38" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:AQ38" xr:uid="{07CD4AC0-49C4-4B86-80BF-22BA39ABB725}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{07CD4AC0-49C4-4B86-80BF-22BA39ABB725}" name="표1" displayName="표1" ref="A1:AQ39" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:AQ39" xr:uid="{07CD4AC0-49C4-4B86-80BF-22BA39ABB725}"/>
   <tableColumns count="43">
     <tableColumn id="1" xr3:uid="{70D73D05-C779-4D87-984C-9925A5D4EBE2}" name="Key"/>
     <tableColumn id="2" xr3:uid="{6C939BEA-81BC-4199-8571-BE159B9E93BD}" name="_memo"/>
@@ -1127,10 +1135,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{315677FB-260A-4651-8343-EA147A10AE96}">
-  <dimension ref="A1:AQ38"/>
+  <dimension ref="A1:AQ39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1678,7 +1686,7 @@
         <v>8</v>
       </c>
       <c r="I5">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="J5">
         <v>105</v>
@@ -1691,7 +1699,7 @@
   IF(표1[[#This Row],[_Condition4]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition4]] &amp; "," &amp; 표1[[#This Row],[_CParam4]] &amp; "," &amp; 표1[[#This Row],[_Function4]] &amp; "," &amp; 표1[[#This Row],[_FParam4]] &amp; "}", ""),
   IF(표1[[#This Row],[_Condition5]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition5]] &amp; "," &amp; 표1[[#This Row],[_CParam5]] &amp; "," &amp; 표1[[#This Row],[_Function5]] &amp; "," &amp; 표1[[#This Row],[_FParam5]] &amp; "}", ""),  IF(표1[[#This Row],[_Condition6]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition6]] &amp; "," &amp; 표1[[#This Row],[_CParam6]] &amp; "," &amp; 표1[[#This Row],[_Function6]] &amp; "," &amp; 표1[[#This Row],[_FParam6]] &amp; "}", ""),  IF(표1[[#This Row],[_Condition7]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition7]] &amp; "," &amp; 표1[[#This Row],[_CParam7]] &amp; "," &amp; 표1[[#This Row],[_Function7]] &amp; "," &amp; 표1[[#This Row],[_FParam7]] &amp; "}", ""),  IF(표1[[#This Row],[_Condition8]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition8]] &amp; "," &amp; 표1[[#This Row],[_CParam8]] &amp; "," &amp; 표1[[#This Row],[_Function8]] &amp; "," &amp; 표1[[#This Row],[_FParam8]] &amp; "}", "")
 ) &amp; "]"</f>
-        <v>[{InputX,1,MoveInputX,1},{Jump,1,MoveY,3},{Jump,0,SetAction,105}]</v>
+        <v>[{InputX,1,MoveInputX,1},{Jump,1,MoveY,6},{Jump,0,SetAction,105}]</v>
       </c>
       <c r="L5" t="s">
         <v>36</v>
@@ -1715,7 +1723,7 @@
         <v>64</v>
       </c>
       <c r="S5">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="T5" t="s">
         <v>42</v>
@@ -1750,7 +1758,7 @@
         <v>0.2</v>
       </c>
       <c r="G6">
-        <v>2</v>
+        <v>4.5</v>
       </c>
       <c r="H6">
         <v>8</v>
@@ -2329,7 +2337,7 @@
         <v>0</v>
       </c>
       <c r="I12">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="J12">
         <v>105</v>
@@ -2342,19 +2350,19 @@
   IF(표1[[#This Row],[_Condition4]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition4]] &amp; "," &amp; 표1[[#This Row],[_CParam4]] &amp; "," &amp; 표1[[#This Row],[_Function4]] &amp; "," &amp; 표1[[#This Row],[_FParam4]] &amp; "}", ""),
   IF(표1[[#This Row],[_Condition5]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition5]] &amp; "," &amp; 표1[[#This Row],[_CParam5]] &amp; "," &amp; 표1[[#This Row],[_Function5]] &amp; "," &amp; 표1[[#This Row],[_FParam5]] &amp; "}", ""),  IF(표1[[#This Row],[_Condition6]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition6]] &amp; "," &amp; 표1[[#This Row],[_CParam6]] &amp; "," &amp; 표1[[#This Row],[_Function6]] &amp; "," &amp; 표1[[#This Row],[_FParam6]] &amp; "}", ""),  IF(표1[[#This Row],[_Condition7]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition7]] &amp; "," &amp; 표1[[#This Row],[_CParam7]] &amp; "," &amp; 표1[[#This Row],[_Function7]] &amp; "," &amp; 표1[[#This Row],[_FParam7]] &amp; "}", ""),  IF(표1[[#This Row],[_Condition8]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition8]] &amp; "," &amp; 표1[[#This Row],[_CParam8]] &amp; "," &amp; 표1[[#This Row],[_Function8]] &amp; "," &amp; 표1[[#This Row],[_FParam8]] &amp; "}", "")
 ) &amp; "]"</f>
-        <v>[{Frame,1,MoveY,18}]</v>
+        <v>[{Frame,0,MoveY,20}]</v>
       </c>
       <c r="L12" t="s">
         <v>55</v>
       </c>
       <c r="M12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N12" t="s">
         <v>64</v>
       </c>
       <c r="O12">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:43" x14ac:dyDescent="0.3">
@@ -3122,7 +3130,7 @@
   IF(표1[[#This Row],[_Condition4]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition4]] &amp; "," &amp; 표1[[#This Row],[_CParam4]] &amp; "," &amp; 표1[[#This Row],[_Function4]] &amp; "," &amp; 표1[[#This Row],[_FParam4]] &amp; "}", ""),
   IF(표1[[#This Row],[_Condition5]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition5]] &amp; "," &amp; 표1[[#This Row],[_CParam5]] &amp; "," &amp; 표1[[#This Row],[_Function5]] &amp; "," &amp; 표1[[#This Row],[_FParam5]] &amp; "}", ""),  IF(표1[[#This Row],[_Condition6]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition6]] &amp; "," &amp; 표1[[#This Row],[_CParam6]] &amp; "," &amp; 표1[[#This Row],[_Function6]] &amp; "," &amp; 표1[[#This Row],[_FParam6]] &amp; "}", ""),  IF(표1[[#This Row],[_Condition7]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition7]] &amp; "," &amp; 표1[[#This Row],[_CParam7]] &amp; "," &amp; 표1[[#This Row],[_Function7]] &amp; "," &amp; 표1[[#This Row],[_FParam7]] &amp; "}", ""),  IF(표1[[#This Row],[_Condition8]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition8]] &amp; "," &amp; 표1[[#This Row],[_CParam8]] &amp; "," &amp; 표1[[#This Row],[_Function8]] &amp; "," &amp; 표1[[#This Row],[_FParam8]] &amp; "}", "")
 ) &amp; "]"</f>
-        <v>[{InputY,1,Stretch,0.2},{InputX,1,MoveInputX,0.05},{Jump,1,MoveY,3},{InputY,0,SetAction,184},{InputY,-1,SetAction,184},{OnLand,1,SetAction,108}]</v>
+        <v>[{InputY,1,Stretch,0.2},{InputX,1,MoveInputX,0.05},{Jump,1,MoveY,3},{Jump,0,SetAction,183},{InputY,0,SetAction,184},{InputY,-1,SetAction,184}]</v>
       </c>
       <c r="L22" t="s">
         <v>38</v>
@@ -3161,7 +3169,7 @@
         <v>3</v>
       </c>
       <c r="X22" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="Y22">
         <v>0</v>
@@ -3170,13 +3178,13 @@
         <v>71</v>
       </c>
       <c r="AA22">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AB22" t="s">
         <v>38</v>
       </c>
       <c r="AC22">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AD22" t="s">
         <v>71</v>
@@ -3185,16 +3193,16 @@
         <v>184</v>
       </c>
       <c r="AF22" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="AG22">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AH22" t="s">
         <v>71</v>
       </c>
       <c r="AI22">
-        <v>108</v>
+        <v>184</v>
       </c>
     </row>
     <row r="23" spans="1:39" x14ac:dyDescent="0.3">
@@ -3889,31 +3897,31 @@
     </row>
     <row r="35" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>701</v>
+        <v>602</v>
       </c>
       <c r="B35" t="s">
-        <v>133</v>
+        <v>164</v>
       </c>
       <c r="C35" t="s">
-        <v>140</v>
+        <v>165</v>
       </c>
       <c r="D35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F35">
         <v>0</v>
       </c>
       <c r="G35">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H35">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I35">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K35" t="str">
         <f>"[" &amp; _xlfn.TEXTJOIN(",", TRUE,
@@ -3923,30 +3931,30 @@
   IF(표1[[#This Row],[_Condition4]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition4]] &amp; "," &amp; 표1[[#This Row],[_CParam4]] &amp; "," &amp; 표1[[#This Row],[_Function4]] &amp; "," &amp; 표1[[#This Row],[_FParam4]] &amp; "}", ""),
   IF(표1[[#This Row],[_Condition5]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition5]] &amp; "," &amp; 표1[[#This Row],[_CParam5]] &amp; "," &amp; 표1[[#This Row],[_Function5]] &amp; "," &amp; 표1[[#This Row],[_FParam5]] &amp; "}", ""),  IF(표1[[#This Row],[_Condition6]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition6]] &amp; "," &amp; 표1[[#This Row],[_CParam6]] &amp; "," &amp; 표1[[#This Row],[_Function6]] &amp; "," &amp; 표1[[#This Row],[_FParam6]] &amp; "}", ""),  IF(표1[[#This Row],[_Condition7]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition7]] &amp; "," &amp; 표1[[#This Row],[_CParam7]] &amp; "," &amp; 표1[[#This Row],[_Function7]] &amp; "," &amp; 표1[[#This Row],[_FParam7]] &amp; "}", ""),  IF(표1[[#This Row],[_Condition8]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition8]] &amp; "," &amp; 표1[[#This Row],[_CParam8]] &amp; "," &amp; 표1[[#This Row],[_Function8]] &amp; "," &amp; 표1[[#This Row],[_FParam8]] &amp; "}", "")
 ) &amp; "]"</f>
-        <v>[{PlayerInSight,1,SetAction,702}]</v>
+        <v>[{Walkable,1,StalkX,-3}]</v>
       </c>
       <c r="L35" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="M35">
         <v>1</v>
       </c>
       <c r="N35" t="s">
-        <v>71</v>
+        <v>148</v>
       </c>
       <c r="O35">
-        <v>702</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="36" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B36" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C36" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -3965,9 +3973,6 @@
       </c>
       <c r="I36">
         <v>0</v>
-      </c>
-      <c r="J36">
-        <v>703</v>
       </c>
       <c r="K36" t="str">
         <f>"[" &amp; _xlfn.TEXTJOIN(",", TRUE,
@@ -3977,48 +3982,51 @@
   IF(표1[[#This Row],[_Condition4]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition4]] &amp; "," &amp; 표1[[#This Row],[_CParam4]] &amp; "," &amp; 표1[[#This Row],[_Function4]] &amp; "," &amp; 표1[[#This Row],[_FParam4]] &amp; "}", ""),
   IF(표1[[#This Row],[_Condition5]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition5]] &amp; "," &amp; 표1[[#This Row],[_CParam5]] &amp; "," &amp; 표1[[#This Row],[_Function5]] &amp; "," &amp; 표1[[#This Row],[_FParam5]] &amp; "}", ""),  IF(표1[[#This Row],[_Condition6]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition6]] &amp; "," &amp; 표1[[#This Row],[_CParam6]] &amp; "," &amp; 표1[[#This Row],[_Function6]] &amp; "," &amp; 표1[[#This Row],[_FParam6]] &amp; "}", ""),  IF(표1[[#This Row],[_Condition7]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition7]] &amp; "," &amp; 표1[[#This Row],[_CParam7]] &amp; "," &amp; 표1[[#This Row],[_Function7]] &amp; "," &amp; 표1[[#This Row],[_FParam7]] &amp; "}", ""),  IF(표1[[#This Row],[_Condition8]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition8]] &amp; "," &amp; 표1[[#This Row],[_CParam8]] &amp; "," &amp; 표1[[#This Row],[_Function8]] &amp; "," &amp; 표1[[#This Row],[_FParam8]] &amp; "}", "")
 ) &amp; "]"</f>
-        <v>[{Frame,-1,MoveInputX,0}]</v>
+        <v>[{PlayerInSight,1,SetAction,702}]</v>
       </c>
       <c r="L36" t="s">
-        <v>55</v>
+        <v>147</v>
       </c>
       <c r="M36">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="N36" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="O36">
-        <v>0</v>
+        <v>702</v>
       </c>
     </row>
     <row r="37" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A37">
+        <v>702</v>
+      </c>
+      <c r="B37" t="s">
+        <v>134</v>
+      </c>
+      <c r="C37" t="s">
+        <v>141</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <v>0</v>
+      </c>
+      <c r="J37">
         <v>703</v>
-      </c>
-      <c r="B37" t="s">
-        <v>136</v>
-      </c>
-      <c r="C37" t="s">
-        <v>142</v>
-      </c>
-      <c r="D37">
-        <v>2</v>
-      </c>
-      <c r="E37">
-        <v>3</v>
-      </c>
-      <c r="F37">
-        <v>0.5</v>
-      </c>
-      <c r="G37">
-        <v>0</v>
-      </c>
-      <c r="H37">
-        <v>12</v>
-      </c>
-      <c r="I37">
-        <v>12</v>
       </c>
       <c r="K37" t="str">
         <f>"[" &amp; _xlfn.TEXTJOIN(",", TRUE,
@@ -4028,66 +4036,30 @@
   IF(표1[[#This Row],[_Condition4]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition4]] &amp; "," &amp; 표1[[#This Row],[_CParam4]] &amp; "," &amp; 표1[[#This Row],[_Function4]] &amp; "," &amp; 표1[[#This Row],[_FParam4]] &amp; "}", ""),
   IF(표1[[#This Row],[_Condition5]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition5]] &amp; "," &amp; 표1[[#This Row],[_CParam5]] &amp; "," &amp; 표1[[#This Row],[_Function5]] &amp; "," &amp; 표1[[#This Row],[_FParam5]] &amp; "}", ""),  IF(표1[[#This Row],[_Condition6]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition6]] &amp; "," &amp; 표1[[#This Row],[_CParam6]] &amp; "," &amp; 표1[[#This Row],[_Function6]] &amp; "," &amp; 표1[[#This Row],[_FParam6]] &amp; "}", ""),  IF(표1[[#This Row],[_Condition7]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition7]] &amp; "," &amp; 표1[[#This Row],[_CParam7]] &amp; "," &amp; 표1[[#This Row],[_Function7]] &amp; "," &amp; 표1[[#This Row],[_FParam7]] &amp; "}", ""),  IF(표1[[#This Row],[_Condition8]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition8]] &amp; "," &amp; 표1[[#This Row],[_CParam8]] &amp; "," &amp; 표1[[#This Row],[_Function8]] &amp; "," &amp; 표1[[#This Row],[_FParam8]] &amp; "}", "")
 ) &amp; "]"</f>
-        <v>[{Frame,1,StalkX,12},{Frame,1,StalkY,12},{Frame,90,SetAction,704},{None,1,StalkX,0.01}]</v>
+        <v>[{Frame,-1,MoveInputX,0}]</v>
       </c>
       <c r="L37" t="s">
         <v>55</v>
       </c>
       <c r="M37">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="N37" t="s">
-        <v>148</v>
+        <v>59</v>
       </c>
       <c r="O37">
-        <v>12</v>
-      </c>
-      <c r="P37" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q37">
-        <v>1</v>
-      </c>
-      <c r="R37" t="s">
-        <v>149</v>
-      </c>
-      <c r="S37">
-        <v>12</v>
-      </c>
-      <c r="T37" t="s">
-        <v>55</v>
-      </c>
-      <c r="U37">
-        <v>90</v>
-      </c>
-      <c r="V37" t="s">
-        <v>71</v>
-      </c>
-      <c r="W37">
-        <v>704</v>
-      </c>
-      <c r="X37" t="s">
-        <v>162</v>
-      </c>
-      <c r="Y37">
-        <v>1</v>
-      </c>
-      <c r="Z37" t="s">
-        <v>148</v>
-      </c>
-      <c r="AA37">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="B38" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C38" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D38">
         <v>2</v>
@@ -4096,16 +4068,16 @@
         <v>3</v>
       </c>
       <c r="F38">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G38">
         <v>0</v>
       </c>
       <c r="H38">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="I38">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="K38" t="str">
         <f>"[" &amp; _xlfn.TEXTJOIN(",", TRUE,
@@ -4115,42 +4087,129 @@
   IF(표1[[#This Row],[_Condition4]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition4]] &amp; "," &amp; 표1[[#This Row],[_CParam4]] &amp; "," &amp; 표1[[#This Row],[_Function4]] &amp; "," &amp; 표1[[#This Row],[_FParam4]] &amp; "}", ""),
   IF(표1[[#This Row],[_Condition5]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition5]] &amp; "," &amp; 표1[[#This Row],[_CParam5]] &amp; "," &amp; 표1[[#This Row],[_Function5]] &amp; "," &amp; 표1[[#This Row],[_FParam5]] &amp; "}", ""),  IF(표1[[#This Row],[_Condition6]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition6]] &amp; "," &amp; 표1[[#This Row],[_CParam6]] &amp; "," &amp; 표1[[#This Row],[_Function6]] &amp; "," &amp; 표1[[#This Row],[_FParam6]] &amp; "}", ""),  IF(표1[[#This Row],[_Condition7]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition7]] &amp; "," &amp; 표1[[#This Row],[_CParam7]] &amp; "," &amp; 표1[[#This Row],[_Function7]] &amp; "," &amp; 표1[[#This Row],[_FParam7]] &amp; "}", ""),  IF(표1[[#This Row],[_Condition8]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition8]] &amp; "," &amp; 표1[[#This Row],[_CParam8]] &amp; "," &amp; 표1[[#This Row],[_Function8]] &amp; "," &amp; 표1[[#This Row],[_FParam8]] &amp; "}", "")
 ) &amp; "]"</f>
-        <v>[{Frame,360,SetAction,703},{None,1,StalkX,0.1},{None,1,StalkY,0.1}]</v>
+        <v>[{Frame,1,StalkX,12},{Frame,1,StalkY,12},{Frame,90,SetAction,704},{None,1,StalkX,0.01}]</v>
       </c>
       <c r="L38" t="s">
         <v>55</v>
       </c>
       <c r="M38">
+        <v>1</v>
+      </c>
+      <c r="N38" t="s">
+        <v>148</v>
+      </c>
+      <c r="O38">
+        <v>12</v>
+      </c>
+      <c r="P38" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q38">
+        <v>1</v>
+      </c>
+      <c r="R38" t="s">
+        <v>149</v>
+      </c>
+      <c r="S38">
+        <v>12</v>
+      </c>
+      <c r="T38" t="s">
+        <v>55</v>
+      </c>
+      <c r="U38">
+        <v>90</v>
+      </c>
+      <c r="V38" t="s">
+        <v>71</v>
+      </c>
+      <c r="W38">
+        <v>704</v>
+      </c>
+      <c r="X38" t="s">
+        <v>162</v>
+      </c>
+      <c r="Y38">
+        <v>1</v>
+      </c>
+      <c r="Z38" t="s">
+        <v>148</v>
+      </c>
+      <c r="AA38">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="39" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>704</v>
+      </c>
+      <c r="B39" t="s">
+        <v>135</v>
+      </c>
+      <c r="C39" t="s">
+        <v>143</v>
+      </c>
+      <c r="D39">
+        <v>2</v>
+      </c>
+      <c r="E39">
+        <v>3</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>3</v>
+      </c>
+      <c r="I39">
+        <v>3</v>
+      </c>
+      <c r="K39" t="str">
+        <f>"[" &amp; _xlfn.TEXTJOIN(",", TRUE,
+  IF(표1[[#This Row],[_Condition1]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition1]] &amp; "," &amp; 표1[[#This Row],[_CParam1]] &amp; "," &amp; 표1[[#This Row],[_Function1]] &amp; "," &amp; 표1[[#This Row],[_FParam1]] &amp; "}", ""),
+  IF(표1[[#This Row],[_Condition2]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition2]] &amp; "," &amp; 표1[[#This Row],[_CParam2]] &amp; "," &amp; 표1[[#This Row],[_Function2]] &amp; "," &amp; 표1[[#This Row],[_FParam2]] &amp; "}", ""),
+  IF(표1[[#This Row],[_Condition3]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition3]] &amp; "," &amp; 표1[[#This Row],[_CParam3]] &amp; "," &amp; 표1[[#This Row],[_Function3]] &amp; "," &amp; 표1[[#This Row],[_FParam3]] &amp; "}", ""),
+  IF(표1[[#This Row],[_Condition4]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition4]] &amp; "," &amp; 표1[[#This Row],[_CParam4]] &amp; "," &amp; 표1[[#This Row],[_Function4]] &amp; "," &amp; 표1[[#This Row],[_FParam4]] &amp; "}", ""),
+  IF(표1[[#This Row],[_Condition5]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition5]] &amp; "," &amp; 표1[[#This Row],[_CParam5]] &amp; "," &amp; 표1[[#This Row],[_Function5]] &amp; "," &amp; 표1[[#This Row],[_FParam5]] &amp; "}", ""),  IF(표1[[#This Row],[_Condition6]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition6]] &amp; "," &amp; 표1[[#This Row],[_CParam6]] &amp; "," &amp; 표1[[#This Row],[_Function6]] &amp; "," &amp; 표1[[#This Row],[_FParam6]] &amp; "}", ""),  IF(표1[[#This Row],[_Condition7]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition7]] &amp; "," &amp; 표1[[#This Row],[_CParam7]] &amp; "," &amp; 표1[[#This Row],[_Function7]] &amp; "," &amp; 표1[[#This Row],[_FParam7]] &amp; "}", ""),  IF(표1[[#This Row],[_Condition8]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition8]] &amp; "," &amp; 표1[[#This Row],[_CParam8]] &amp; "," &amp; 표1[[#This Row],[_Function8]] &amp; "," &amp; 표1[[#This Row],[_FParam8]] &amp; "}", "")
+) &amp; "]"</f>
+        <v>[{Frame,360,SetAction,703},{None,1,StalkX,0.1},{None,1,StalkY,0.1}]</v>
+      </c>
+      <c r="L39" t="s">
+        <v>55</v>
+      </c>
+      <c r="M39">
         <v>360</v>
       </c>
-      <c r="N38" t="s">
-        <v>71</v>
-      </c>
-      <c r="O38">
+      <c r="N39" t="s">
+        <v>71</v>
+      </c>
+      <c r="O39">
         <v>703</v>
       </c>
-      <c r="P38" t="s">
+      <c r="P39" t="s">
         <v>162</v>
       </c>
-      <c r="Q38">
-        <v>1</v>
-      </c>
-      <c r="R38" t="s">
+      <c r="Q39">
+        <v>1</v>
+      </c>
+      <c r="R39" t="s">
         <v>148</v>
       </c>
-      <c r="S38">
+      <c r="S39">
         <v>0.1</v>
       </c>
-      <c r="T38" t="s">
+      <c r="T39" t="s">
         <v>162</v>
       </c>
-      <c r="U38">
-        <v>1</v>
-      </c>
-      <c r="V38" t="s">
+      <c r="U39">
+        <v>1</v>
+      </c>
+      <c r="V39" t="s">
         <v>149</v>
       </c>
-      <c r="W38">
+      <c r="W39">
         <v>0.1</v>
       </c>
     </row>
@@ -4168,13 +4227,13 @@
           <x14:formula1>
             <xm:f>_helper!$B:$B</xm:f>
           </x14:formula1>
-          <xm:sqref>AP3 AL8 AL21:AL23 AL2:AL3 AD2:AD38 N2:N38 AH2:AH38 R2:R38 Z2:Z38 V2:V38</xm:sqref>
+          <xm:sqref>AP3 AL8 AL2:AL3 AL21:AL23 Z2:Z39 AD2:AD39 AH2:AH39 N2:N39 V2:V39 R2:R39</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{38EFAF22-778F-4724-863A-ECD1104B256A}">
           <x14:formula1>
             <xm:f>_helper!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>AN3 AJ8 AJ21:AJ23 AJ2:AJ3 AB2:AB38 L2:L38 AF2:AF38 P2:P38 X2:X38 T2:T38</xm:sqref>
+          <xm:sqref>AN3 AJ8 AJ2:AJ3 AJ21:AJ23 X2:X39 AB2:AB39 AF2:AF39 L2:L39 T2:T39 P2:P39</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
[ISSUE-B20] Fix jump strechspeed
</commit_message>
<xml_diff>
--- a/RunInBoots/Assets/Excel/ActionTable.xlsx
+++ b/RunInBoots/Assets/Excel/ActionTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeonhyeonseong/Unity/team-project-for-2024-fall-swpp-team-05/RunInBoots/Assets/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{148A0A18-E424-E343-8E6E-FB940C987EBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36247F25-E9F1-8549-9C79-DBF8E0945A8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="500" windowWidth="29040" windowHeight="15720" xr2:uid="{D47B4964-B3F8-4260-96F1-09DFF1E3D63F}"/>
   </bookViews>
@@ -1137,8 +1137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{315677FB-260A-4651-8343-EA147A10AE96}">
   <dimension ref="A1:AQ39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B5" zoomScale="167" workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="167" workbookViewId="0">
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3179,7 +3179,7 @@
   IF(표1[[#This Row],[_Condition4]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition4]] &amp; "," &amp; 표1[[#This Row],[_CParam4]] &amp; "," &amp; 표1[[#This Row],[_Function4]] &amp; "," &amp; 표1[[#This Row],[_FParam4]] &amp; "}", ""),
   IF(표1[[#This Row],[_Condition5]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition5]] &amp; "," &amp; 표1[[#This Row],[_CParam5]] &amp; "," &amp; 표1[[#This Row],[_Function5]] &amp; "," &amp; 표1[[#This Row],[_FParam5]] &amp; "}", ""),  IF(표1[[#This Row],[_Condition6]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition6]] &amp; "," &amp; 표1[[#This Row],[_CParam6]] &amp; "," &amp; 표1[[#This Row],[_Function6]] &amp; "," &amp; 표1[[#This Row],[_FParam6]] &amp; "}", ""),  IF(표1[[#This Row],[_Condition7]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition7]] &amp; "," &amp; 표1[[#This Row],[_CParam7]] &amp; "," &amp; 표1[[#This Row],[_Function7]] &amp; "," &amp; 표1[[#This Row],[_FParam7]] &amp; "}", ""),  IF(표1[[#This Row],[_Condition8]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition8]] &amp; "," &amp; 표1[[#This Row],[_CParam8]] &amp; "," &amp; 표1[[#This Row],[_Function8]] &amp; "," &amp; 표1[[#This Row],[_FParam8]] &amp; "}", "")
 ) &amp; "]"</f>
-        <v>[{InputY,1,Stretch,0.01},{InputX,1,MoveInputX,0.05},{Jump,1,MoveY,3},{Jump,0,SetAction,183},{InputY,0,SetAction,184},{InputY,-1,SetAction,184}]</v>
+        <v>[{InputY,1,Stretch,0.05},{InputX,1,MoveInputX,0.05},{Jump,1,MoveY,3},{Jump,0,SetAction,183},{InputY,0,SetAction,184},{InputY,-1,SetAction,184}]</v>
       </c>
       <c r="L22" t="s">
         <v>38</v>
@@ -3191,7 +3191,7 @@
         <v>153</v>
       </c>
       <c r="O22">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="P22" t="s">
         <v>36</v>
@@ -3290,7 +3290,7 @@
   IF(표1[[#This Row],[_Condition4]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition4]] &amp; "," &amp; 표1[[#This Row],[_CParam4]] &amp; "," &amp; 표1[[#This Row],[_Function4]] &amp; "," &amp; 표1[[#This Row],[_FParam4]] &amp; "}", ""),
   IF(표1[[#This Row],[_Condition5]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition5]] &amp; "," &amp; 표1[[#This Row],[_CParam5]] &amp; "," &amp; 표1[[#This Row],[_Function5]] &amp; "," &amp; 표1[[#This Row],[_FParam5]] &amp; "}", ""),  IF(표1[[#This Row],[_Condition6]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition6]] &amp; "," &amp; 표1[[#This Row],[_CParam6]] &amp; "," &amp; 표1[[#This Row],[_Function6]] &amp; "," &amp; 표1[[#This Row],[_FParam6]] &amp; "}", ""),  IF(표1[[#This Row],[_Condition7]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition7]] &amp; "," &amp; 표1[[#This Row],[_CParam7]] &amp; "," &amp; 표1[[#This Row],[_Function7]] &amp; "," &amp; 표1[[#This Row],[_FParam7]] &amp; "}", ""),  IF(표1[[#This Row],[_Condition8]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition8]] &amp; "," &amp; 표1[[#This Row],[_CParam8]] &amp; "," &amp; 표1[[#This Row],[_Function8]] &amp; "," &amp; 표1[[#This Row],[_FParam8]] &amp; "}", "")
 ) &amp; "]"</f>
-        <v>[{InputY,1,Stretch,0.01},{InputX,1,MoveInputX,0.05},{InputY,0,SetAction,184},{InputY,-1,SetAction,184},{OnLand,1,SetAction,108}]</v>
+        <v>[{InputY,1,Stretch,0.05},{InputX,1,MoveInputX,0.05},{InputY,0,SetAction,184},{InputY,-1,SetAction,184},{OnLand,1,SetAction,108}]</v>
       </c>
       <c r="L23" t="s">
         <v>38</v>
@@ -3302,7 +3302,7 @@
         <v>153</v>
       </c>
       <c r="O23">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="P23" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
[ISSUE-B40] Fix jump sound condition in action system
</commit_message>
<xml_diff>
--- a/RunInBoots/Assets/Excel/ActionTable.xlsx
+++ b/RunInBoots/Assets/Excel/ActionTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paul1\OneDrive\문서\Git\team-project-for-2024-fall-swpp-team-05\RunInBoots\Assets\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yuye2\SWPP2024\team-project-for-2024-fall-swpp-team-05\RunInBoots\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D281D06C-B92B-4C39-BBD0-78D3FFDA2B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9094FF3F-FD7B-4EB0-99AE-BBF352496E52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-165" windowWidth="29040" windowHeight="15720" xr2:uid="{D47B4964-B3F8-4260-96F1-09DFF1E3D63F}"/>
+    <workbookView xWindow="7140" yWindow="495" windowWidth="15720" windowHeight="14985" xr2:uid="{D47B4964-B3F8-4260-96F1-09DFF1E3D63F}"/>
   </bookViews>
   <sheets>
     <sheet name="Actions" sheetId="1" r:id="rId1"/>
@@ -20,17 +20,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -44,10 +33,20 @@
   <commentList>
     <comment ref="S13" authorId="0" shapeId="0" xr:uid="{E66A3162-0F90-431A-9409-B94D42850838}">
       <text>
-        <t>[스레드 댓글]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="맑은 고딕"/>
+            <family val="2"/>
+            <charset val="129"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[스레드 댓글]
 사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
 댓글:
     넙버링 맞추기용 1 + 유닛 키 01 +카테고리 00 + 인덱스 001</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -55,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="173">
   <si>
     <t>Key</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -691,6 +690,10 @@
   </si>
   <si>
     <t>Empty</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IsStretchingStart</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -737,15 +740,12 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1164,8 +1164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{315677FB-260A-4651-8343-EA147A10AE96}">
   <dimension ref="A1:AQ43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="Q39" sqref="Q39"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
+      <selection activeCell="AJ9" sqref="AJ9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2089,7 +2089,7 @@
   IF(표1[[#This Row],[_Condition4]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition4]] &amp; "," &amp; 표1[[#This Row],[_CParam4]] &amp; "," &amp; 표1[[#This Row],[_Function4]] &amp; "," &amp; 표1[[#This Row],[_FParam4]] &amp; "}", ""),
   IF(표1[[#This Row],[_Condition5]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition5]] &amp; "," &amp; 표1[[#This Row],[_CParam5]] &amp; "," &amp; 표1[[#This Row],[_Function5]] &amp; "," &amp; 표1[[#This Row],[_FParam5]] &amp; "}", ""),  IF(표1[[#This Row],[_Condition6]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition6]] &amp; "," &amp; 표1[[#This Row],[_CParam6]] &amp; "," &amp; 표1[[#This Row],[_Function6]] &amp; "," &amp; 표1[[#This Row],[_FParam6]] &amp; "}", ""),  IF(표1[[#This Row],[_Condition7]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition7]] &amp; "," &amp; 표1[[#This Row],[_CParam7]] &amp; "," &amp; 표1[[#This Row],[_Function7]] &amp; "," &amp; 표1[[#This Row],[_FParam7]] &amp; "}", ""),  IF(표1[[#This Row],[_Condition8]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition8]] &amp; "," &amp; 표1[[#This Row],[_CParam8]] &amp; "," &amp; 표1[[#This Row],[_Function8]] &amp; "," &amp; 표1[[#This Row],[_FParam8]] &amp; "}", "")
 ) &amp; "]"</f>
-        <v>[{InputY,1,Stretch,0.2},{InputX,1,SetAction,181},{InputY,0,SetAction,184},{InputY,-1,SetAction,184},{OnLand,0,SetAction,183},{JumpValid,1,SetAction,182},{Frame,0,Spawn,10100002}]</v>
+        <v>[{InputY,1,Stretch,0.2},{InputX,1,SetAction,181},{InputY,0,SetAction,184},{InputY,-1,SetAction,184},{OnLand,0,SetAction,183},{JumpValid,1,SetAction,182},{IsStretchingStart,1,Spawn,10100002}]</v>
       </c>
       <c r="L9" t="s">
         <v>38</v>
@@ -2164,10 +2164,10 @@
         <v>182</v>
       </c>
       <c r="AJ9" t="s">
-        <v>56</v>
+        <v>172</v>
       </c>
       <c r="AK9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL9" t="s">
         <v>68</v>
@@ -4229,7 +4229,7 @@
       <c r="I39">
         <v>0</v>
       </c>
-      <c r="K39" s="2" t="str">
+      <c r="K39" t="str">
         <f>"[" &amp; _xlfn.TEXTJOIN(",", TRUE,
   IF(표1[[#This Row],[_Condition1]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition1]] &amp; "," &amp; 표1[[#This Row],[_CParam1]] &amp; "," &amp; 표1[[#This Row],[_Function1]] &amp; "," &amp; 표1[[#This Row],[_FParam1]] &amp; "}", ""),
   IF(표1[[#This Row],[_Condition2]]&lt;&gt;"", "{" &amp; 표1[[#This Row],[_Condition2]] &amp; "," &amp; 표1[[#This Row],[_CParam2]] &amp; "," &amp; 표1[[#This Row],[_Function2]] &amp; "," &amp; 표1[[#This Row],[_FParam2]] &amp; "}", ""),

</xml_diff>